<commit_message>
unfreeze panes on schedule
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmac\Google Drive\courses\data-structures\schedule\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmac\git\dickinson-comp232.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF91518C-1830-4D52-BB55-68315F164CAD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A9308B-7AD9-4DB7-BB84-E68E18140EB4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -639,23 +639,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1000,10 +1000,8 @@
   </sheetPr>
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="60" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection activeCell="D1" sqref="D1"/>
-      <selection pane="topRight" activeCell="D10" sqref="D10:D11"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1015,7 +1013,7 @@
     <col min="5" max="5" width="10.5703125" style="18" customWidth="1"/>
     <col min="6" max="6" width="12" style="11" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" style="13" customWidth="1"/>
-    <col min="8" max="8" width="51.7109375" style="30" customWidth="1"/>
+    <col min="8" max="8" width="51.7109375" style="28" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="14"/>
   </cols>
   <sheetData>
@@ -1065,7 +1063,7 @@
       <c r="G2" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="29" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1078,7 +1076,7 @@
         <f>C2+2</f>
         <v>44441</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="33" t="s">
         <v>43</v>
       </c>
       <c r="E3" s="7" t="s">
@@ -1088,7 +1086,7 @@
       <c r="G3" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="H3" s="31" t="s">
+      <c r="H3" s="29" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1105,7 +1103,7 @@
         <f>C2+7</f>
         <v>44446</v>
       </c>
-      <c r="D4" s="28"/>
+      <c r="D4" s="33"/>
       <c r="E4" s="7" t="s">
         <v>17</v>
       </c>
@@ -1115,7 +1113,7 @@
       <c r="G4" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="H4" s="31" t="s">
+      <c r="H4" s="29" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1129,7 +1127,7 @@
         <f>C3+7</f>
         <v>44448</v>
       </c>
-      <c r="D5" s="28"/>
+      <c r="D5" s="33"/>
       <c r="E5" s="7" t="s">
         <v>18</v>
       </c>
@@ -1137,7 +1135,7 @@
       <c r="G5" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H5" s="31" t="s">
+      <c r="H5" s="29" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1154,7 +1152,7 @@
         <f t="shared" ref="C6:C31" si="2">C4+7</f>
         <v>44453</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="33" t="s">
         <v>44</v>
       </c>
       <c r="E6" s="7" t="s">
@@ -1166,7 +1164,7 @@
       <c r="G6" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="H6" s="31" t="s">
+      <c r="H6" s="29" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1180,7 +1178,7 @@
         <f t="shared" si="2"/>
         <v>44455</v>
       </c>
-      <c r="D7" s="28"/>
+      <c r="D7" s="33"/>
       <c r="E7" s="7" t="s">
         <v>20</v>
       </c>
@@ -1188,7 +1186,7 @@
       <c r="G7" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="H7" s="31" t="s">
+      <c r="H7" s="29" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1205,7 +1203,7 @@
         <f t="shared" si="2"/>
         <v>44460</v>
       </c>
-      <c r="D8" s="28"/>
+      <c r="D8" s="33"/>
       <c r="E8" s="7" t="s">
         <v>21</v>
       </c>
@@ -1213,7 +1211,7 @@
       <c r="G8" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="H8" s="31" t="s">
+      <c r="H8" s="29" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1239,7 +1237,7 @@
       <c r="G9" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="H9" s="32" t="s">
+      <c r="H9" s="30" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1256,7 +1254,7 @@
         <f t="shared" si="2"/>
         <v>44467</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="33" t="s">
         <v>46</v>
       </c>
       <c r="E10" s="7" t="s">
@@ -1266,7 +1264,7 @@
       <c r="G10" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="H10" s="31" t="s">
+      <c r="H10" s="29" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1280,7 +1278,7 @@
         <f t="shared" si="2"/>
         <v>44469</v>
       </c>
-      <c r="D11" s="28"/>
+      <c r="D11" s="33"/>
       <c r="E11" s="7" t="s">
         <v>24</v>
       </c>
@@ -1288,7 +1286,7 @@
       <c r="G11" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="H11" s="31" t="s">
+      <c r="H11" s="29" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1305,15 +1303,15 @@
         <f t="shared" si="2"/>
         <v>44474</v>
       </c>
-      <c r="D12" s="29" t="s">
+      <c r="D12" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="29"/>
+      <c r="E12" s="32"/>
       <c r="F12" s="19" t="s">
         <v>78</v>
       </c>
       <c r="G12" s="9"/>
-      <c r="H12" s="31"/>
+      <c r="H12" s="29"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="20"/>
@@ -1325,13 +1323,13 @@
         <f t="shared" si="2"/>
         <v>44476</v>
       </c>
-      <c r="D13" s="29" t="s">
+      <c r="D13" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="29"/>
+      <c r="E13" s="32"/>
       <c r="F13" s="7"/>
       <c r="G13" s="9"/>
-      <c r="H13" s="31"/>
+      <c r="H13" s="29"/>
     </row>
     <row r="14" spans="1:8" ht="27.75" x14ac:dyDescent="0.25">
       <c r="A14" s="20">
@@ -1346,7 +1344,7 @@
         <f t="shared" si="2"/>
         <v>44481</v>
       </c>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="33" t="s">
         <v>47</v>
       </c>
       <c r="E14" s="7" t="s">
@@ -1358,7 +1356,7 @@
       <c r="G14" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="H14" s="31" t="s">
+      <c r="H14" s="29" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1372,7 +1370,7 @@
         <f t="shared" si="2"/>
         <v>44483</v>
       </c>
-      <c r="D15" s="28"/>
+      <c r="D15" s="33"/>
       <c r="E15" s="7" t="s">
         <v>26</v>
       </c>
@@ -1380,7 +1378,7 @@
       <c r="G15" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="H15" s="31" t="s">
+      <c r="H15" s="29" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1397,13 +1395,13 @@
         <f t="shared" si="2"/>
         <v>44488</v>
       </c>
-      <c r="D16" s="28"/>
-      <c r="E16" s="29" t="s">
+      <c r="D16" s="33"/>
+      <c r="E16" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="29"/>
+      <c r="F16" s="32"/>
       <c r="G16" s="9"/>
-      <c r="H16" s="31"/>
+      <c r="H16" s="29"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="20"/>
@@ -1415,7 +1413,7 @@
         <f t="shared" si="2"/>
         <v>44490</v>
       </c>
-      <c r="D17" s="28" t="s">
+      <c r="D17" s="33" t="s">
         <v>48</v>
       </c>
       <c r="E17" s="7" t="s">
@@ -1427,7 +1425,7 @@
       <c r="G17" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="H17" s="31" t="s">
+      <c r="H17" s="29" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1444,7 +1442,7 @@
         <f t="shared" si="2"/>
         <v>44495</v>
       </c>
-      <c r="D18" s="28"/>
+      <c r="D18" s="33"/>
       <c r="E18" s="7" t="s">
         <v>28</v>
       </c>
@@ -1452,7 +1450,7 @@
       <c r="G18" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="H18" s="31" t="s">
+      <c r="H18" s="29" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1466,7 +1464,7 @@
         <f t="shared" si="2"/>
         <v>44497</v>
       </c>
-      <c r="D19" s="28"/>
+      <c r="D19" s="33"/>
       <c r="E19" s="7" t="s">
         <v>29</v>
       </c>
@@ -1474,7 +1472,7 @@
       <c r="G19" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H19" s="31" t="s">
+      <c r="H19" s="29" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1491,7 +1489,7 @@
         <f t="shared" si="2"/>
         <v>44502</v>
       </c>
-      <c r="D20" s="28" t="s">
+      <c r="D20" s="33" t="s">
         <v>49</v>
       </c>
       <c r="E20" s="7" t="s">
@@ -1503,7 +1501,7 @@
       <c r="G20" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="H20" s="31" t="s">
+      <c r="H20" s="29" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1517,7 +1515,7 @@
         <f t="shared" si="2"/>
         <v>44504</v>
       </c>
-      <c r="D21" s="28"/>
+      <c r="D21" s="33"/>
       <c r="E21" s="7" t="s">
         <v>31</v>
       </c>
@@ -1525,7 +1523,7 @@
       <c r="G21" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="H21" s="31" t="s">
+      <c r="H21" s="29" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1542,15 +1540,15 @@
         <f t="shared" si="2"/>
         <v>44509</v>
       </c>
-      <c r="D22" s="29" t="s">
+      <c r="D22" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E22" s="29"/>
+      <c r="E22" s="32"/>
       <c r="F22" s="19" t="s">
         <v>79</v>
       </c>
       <c r="G22" s="9"/>
-      <c r="H22" s="31"/>
+      <c r="H22" s="29"/>
     </row>
     <row r="23" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20"/>
@@ -1562,13 +1560,13 @@
         <f t="shared" si="2"/>
         <v>44511</v>
       </c>
-      <c r="D23" s="29" t="s">
+      <c r="D23" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="E23" s="29"/>
+      <c r="E23" s="32"/>
       <c r="F23" s="8"/>
       <c r="G23" s="9"/>
-      <c r="H23" s="31"/>
+      <c r="H23" s="29"/>
     </row>
     <row r="24" spans="1:8" ht="27.75" x14ac:dyDescent="0.25">
       <c r="A24" s="20">
@@ -1583,7 +1581,7 @@
         <f t="shared" si="2"/>
         <v>44516</v>
       </c>
-      <c r="D24" s="28" t="s">
+      <c r="D24" s="33" t="s">
         <v>50</v>
       </c>
       <c r="E24" s="7" t="s">
@@ -1595,7 +1593,7 @@
       <c r="G24" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="H24" s="33" t="s">
+      <c r="H24" s="31" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1609,7 +1607,7 @@
         <f t="shared" si="2"/>
         <v>44518</v>
       </c>
-      <c r="D25" s="28"/>
+      <c r="D25" s="33"/>
       <c r="E25" s="7" t="s">
         <v>33</v>
       </c>
@@ -1617,7 +1615,7 @@
       <c r="G25" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="H25" s="31" t="s">
+      <c r="H25" s="29" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1634,7 +1632,7 @@
         <f t="shared" si="2"/>
         <v>44523</v>
       </c>
-      <c r="D26" s="28" t="s">
+      <c r="D26" s="33" t="s">
         <v>51</v>
       </c>
       <c r="E26" s="7" t="s">
@@ -1646,7 +1644,7 @@
       <c r="G26" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="H26" s="31" t="s">
+      <c r="H26" s="29" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1660,13 +1658,13 @@
         <f t="shared" si="2"/>
         <v>44525</v>
       </c>
-      <c r="D27" s="28"/>
-      <c r="E27" s="29" t="s">
+      <c r="D27" s="33"/>
+      <c r="E27" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="F27" s="29"/>
+      <c r="F27" s="32"/>
       <c r="G27" s="9"/>
-      <c r="H27" s="31"/>
+      <c r="H27" s="29"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="20">
@@ -1681,7 +1679,7 @@
         <f t="shared" si="2"/>
         <v>44530</v>
       </c>
-      <c r="D28" s="28"/>
+      <c r="D28" s="33"/>
       <c r="E28" s="7" t="s">
         <v>35</v>
       </c>
@@ -1689,7 +1687,7 @@
       <c r="G28" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H28" s="31" t="s">
+      <c r="H28" s="29" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1703,7 +1701,7 @@
         <f t="shared" si="2"/>
         <v>44532</v>
       </c>
-      <c r="D29" s="28" t="s">
+      <c r="D29" s="33" t="s">
         <v>52</v>
       </c>
       <c r="E29" s="7" t="s">
@@ -1715,7 +1713,7 @@
       <c r="G29" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="H29" s="31" t="s">
+      <c r="H29" s="29" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1732,7 +1730,7 @@
         <f t="shared" si="2"/>
         <v>44537</v>
       </c>
-      <c r="D30" s="28"/>
+      <c r="D30" s="33"/>
       <c r="E30" s="7" t="s">
         <v>37</v>
       </c>
@@ -1740,7 +1738,7 @@
       <c r="G30" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H30" s="31" t="s">
+      <c r="H30" s="29" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1754,13 +1752,13 @@
         <f t="shared" si="2"/>
         <v>44539</v>
       </c>
-      <c r="D31" s="29" t="s">
+      <c r="D31" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E31" s="29"/>
+      <c r="E31" s="32"/>
       <c r="F31" s="7"/>
       <c r="G31" s="9"/>
-      <c r="H31" s="31"/>
+      <c r="H31" s="29"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="20"/>
@@ -1776,7 +1774,7 @@
         <v>14</v>
       </c>
       <c r="G32" s="9"/>
-      <c r="H32" s="31"/>
+      <c r="H32" s="29"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="20"/>
@@ -1786,13 +1784,13 @@
       <c r="C33" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="D33" s="29" t="s">
+      <c r="D33" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="E33" s="29"/>
+      <c r="E33" s="32"/>
       <c r="F33" s="7"/>
       <c r="G33" s="9"/>
-      <c r="H33" s="31"/>
+      <c r="H33" s="29"/>
     </row>
     <row r="34" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F34" s="25"/>
@@ -1800,19 +1798,19 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="D3:D5"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="D14:D16"/>
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="D26:D28"/>
     <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D3:D5"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="D20:D21"/>
     <mergeCell ref="D24:D25"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="D23:E23"/>
     <mergeCell ref="D31:E31"/>

</xml_diff>